<commit_message>
feat: Add modern KPI dashboard and enhance terminal output
Co-authored-by: touyboateng339 <touyboateng339@gmail.com>
</commit_message>
<xml_diff>
--- a/reports/report.xlsx
+++ b/reports/report.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sales Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Summary Statistics" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -488,4 +489,110 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Sales</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2875</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>std</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>853.9125638299665</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>25%</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2375</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>75%</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>3250</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>